<commit_message>
Doc: use more consistent language wrt. trainers
</commit_message>
<xml_diff>
--- a/sphinx-doc/source/_static/tracing/training/cat-training-pipeline.xlsx
+++ b/sphinx-doc/source/_static/tracing/training/cat-training-pipeline.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t xml:space="preserve">Neuron name</t>
   </si>
@@ -256,67 +256,13 @@
     <t xml:space="preserve">Review</t>
   </si>
   <si>
-    <t xml:space="preserve">Soon</t>
+    <t xml:space="preserve">Trainee A</t>
   </si>
   <si>
-    <t xml:space="preserve">Laurie</t>
+    <t xml:space="preserve">Trainee B</t>
   </si>
   <si>
-    <t xml:space="preserve">Austin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                              </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chris</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                         </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                               </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Padideh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maggie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marisa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cullen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tansy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     </t>
+    <t xml:space="preserve">Trainee C</t>
   </si>
   <si>
     <t xml:space="preserve">INSTRUCTIONS</t>
@@ -346,7 +292,7 @@
     <t xml:space="preserve">ex. CAT L2-4 LR</t>
   </si>
   <si>
-    <t xml:space="preserve">ta</t>
+    <t xml:space="preserve">Confidence intervals:</t>
   </si>
   <si>
     <t xml:space="preserve">Tracing deleted for given trainee</t>
@@ -371,6 +317,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve">don't add # 5 to node</t>
@@ -433,13 +382,13 @@
     <t xml:space="preserve">Trainee - Pick next neuron from list</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruchi - Review completed neuron</t>
+    <t xml:space="preserve">Trainer - Review completed neuron</t>
   </si>
   <si>
     <t xml:space="preserve">*Trainees should ask questions if confused about where to stop</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruchi - Update progress sheet</t>
+    <t xml:space="preserve">Trainer - Update progress sheet</t>
   </si>
   <si>
     <t xml:space="preserve">*USE uncertain tags when confused about anything</t>
@@ -456,7 +405,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -503,19 +452,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="0"/>
     </font>
@@ -647,7 +583,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,38 +680,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -789,6 +693,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -808,11 +716,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -897,15 +805,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AD1007"/>
+  <dimension ref="A1:AD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L30" activeCellId="0" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.86"/>
@@ -924,6 +832,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="21" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1279,7 +1188,7 @@
       <c r="AC5" s="8"/>
       <c r="AD5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>78</v>
       </c>
@@ -1382,32 +1291,18 @@
       <c r="AD8" s="23"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="24"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="23"/>
@@ -1420,34 +1315,18 @@
       <c r="AD9" s="23"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="S10" s="24"/>
-      <c r="T10" s="24"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="24"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="23"/>
@@ -1460,411 +1339,337 @@
       <c r="AD10" s="23"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="Q13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="O14" s="7"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="27"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="23"/>
-      <c r="Y11" s="23"/>
-      <c r="Z11" s="23"/>
-      <c r="AA11" s="23"/>
-      <c r="AB11" s="23"/>
-      <c r="AC11" s="23"/>
-      <c r="AD11" s="23"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="26" t="s">
-        <v>85</v>
+      <c r="D15" s="23"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="29" t="n">
+        <v>5</v>
       </c>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="23"/>
-      <c r="X12" s="23"/>
-      <c r="Y12" s="23"/>
-      <c r="Z12" s="23"/>
-      <c r="AA12" s="23"/>
-      <c r="AB12" s="23"/>
-      <c r="AC12" s="23"/>
-      <c r="AD12" s="23"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
+      <c r="I15" s="29" t="n">
+        <v>4</v>
+      </c>
+      <c r="J15" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="L15" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="Q15" s="7"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="24"/>
-      <c r="S13" s="24"/>
-      <c r="T13" s="24"/>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="23"/>
-      <c r="X13" s="23"/>
-      <c r="Y13" s="23"/>
-      <c r="Z13" s="23"/>
-      <c r="AA13" s="23"/>
-      <c r="AB13" s="23"/>
-      <c r="AC13" s="23"/>
-      <c r="AD13" s="23"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="27"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="23"/>
-      <c r="X14" s="23"/>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="23"/>
-      <c r="AC14" s="23"/>
-      <c r="AD14" s="23"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="D16" s="23"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="27"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24" t="s">
-        <v>85</v>
+      <c r="H16" s="32" t="n">
+        <v>1</v>
       </c>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="23"/>
-      <c r="X15" s="23"/>
-      <c r="Y15" s="23"/>
-      <c r="Z15" s="23"/>
-      <c r="AA15" s="23"/>
-      <c r="AB15" s="23"/>
-      <c r="AC15" s="23"/>
-      <c r="AD15" s="23"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="I16" s="32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="J16" s="32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K16" s="32" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="L16" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
-      <c r="Q16" s="27"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="23"/>
-      <c r="X16" s="23"/>
-      <c r="Y16" s="23"/>
-      <c r="Z16" s="23"/>
-      <c r="AA16" s="23"/>
-      <c r="AB16" s="23"/>
-      <c r="AC16" s="23"/>
-      <c r="AD16" s="23"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="23"/>
-      <c r="X17" s="23"/>
-      <c r="Y17" s="23"/>
-      <c r="Z17" s="23"/>
-      <c r="AA17" s="23"/>
-      <c r="AB17" s="23"/>
-      <c r="AC17" s="23"/>
-      <c r="AD17" s="23"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="6" t="s">
+      <c r="D17" s="23"/>
+      <c r="E17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="32" t="s">
-        <v>85</v>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="L18" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="23"/>
-      <c r="X18" s="23"/>
-      <c r="Y18" s="23"/>
-      <c r="Z18" s="23"/>
-      <c r="AA18" s="23"/>
-      <c r="AB18" s="23"/>
-      <c r="AC18" s="23"/>
-      <c r="AD18" s="23"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>109</v>
+      </c>
       <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="32"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="32"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="23"/>
-      <c r="X20" s="23"/>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
-      <c r="AD20" s="23"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
+      <c r="A21" s="7" t="s">
+        <v>113</v>
+      </c>
       <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="32"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="7"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-      <c r="Z21" s="23"/>
-      <c r="AA21" s="23"/>
-      <c r="AB21" s="23"/>
-      <c r="AC21" s="23"/>
-      <c r="AD21" s="23"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="33" t="s">
-        <v>99</v>
+      <c r="A22" s="7" t="s">
+        <v>116</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="34" t="s">
-        <v>100</v>
+      <c r="A23" s="7" t="s">
+        <v>119</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="6" t="s">
-        <v>102</v>
-      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="35" t="s">
-        <v>103</v>
+      <c r="A24" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
       <c r="G24" s="6" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -1874,88 +1679,65 @@
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="s">
-        <v>106</v>
+      <c r="A25" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="7" t="s">
-        <v>107</v>
-      </c>
+      <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="6" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
       <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="19" t="s">
-        <v>109</v>
-      </c>
       <c r="B26" s="7"/>
-      <c r="C26" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="23"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
-      <c r="H26" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="I26" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="J26" s="36" t="n">
-        <v>3</v>
-      </c>
-      <c r="K26" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="L26" s="36" t="n">
-        <v>1</v>
-      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
-        <v>111</v>
-      </c>
       <c r="B27" s="7"/>
-      <c r="C27" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D27" s="23"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="38" t="s">
-        <v>113</v>
+      <c r="G27" s="7" t="s">
+        <v>124</v>
       </c>
-      <c r="H27" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="I27" s="39" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="J27" s="39" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K27" s="39" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="L27" s="39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" s="7" t="s">
-        <v>114</v>
-      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
@@ -1963,126 +1745,83 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="7"/>
-      <c r="C28" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" s="23"/>
-      <c r="E28" s="7" t="s">
-        <v>116</v>
-      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I28" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="K28" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="L28" s="7" t="s">
-        <v>121</v>
-      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="40" t="s">
-        <v>123</v>
-      </c>
-      <c r="I29" s="40" t="s">
-        <v>124</v>
-      </c>
-      <c r="J29" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="K29" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="L29" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="M29" s="7"/>
-      <c r="N29" s="7"/>
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7"/>
+      <c r="AC29" s="7"/>
+      <c r="AD29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="7"/>
-      <c r="N31" s="7"/>
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>130</v>
-      </c>
       <c r="B32" s="7"/>
-      <c r="D32" s="23"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
-      <c r="G32" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>132</v>
-      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
@@ -2092,22 +1831,28 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+      <c r="AA32" s="23"/>
+      <c r="AB32" s="23"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="23"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>133</v>
-      </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
-      <c r="G33" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>135</v>
-      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
@@ -2117,16 +1862,28 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+      <c r="AA33" s="23"/>
+      <c r="AB33" s="23"/>
+      <c r="AC33" s="23"/>
+      <c r="AD33" s="23"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-      <c r="H34" s="32"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
@@ -2136,18 +1893,28 @@
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
+      <c r="AA34" s="23"/>
+      <c r="AB34" s="23"/>
+      <c r="AC34" s="23"/>
+      <c r="AD34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>137</v>
-      </c>
+      <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
-      <c r="G35" s="6" t="s">
-        <v>138</v>
-      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -2158,19 +1925,28 @@
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="23"/>
+      <c r="AA35" s="23"/>
+      <c r="AB35" s="23"/>
+      <c r="AC35" s="23"/>
+      <c r="AD35" s="23"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>139</v>
-      </c>
+      <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
-      <c r="G36" s="6" t="s">
-        <v>140</v>
-      </c>
+      <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
@@ -2181,8 +1957,22 @@
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="23"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -2199,16 +1989,28 @@
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="7"/>
+      <c r="W37" s="23"/>
+      <c r="X37" s="23"/>
+      <c r="Y37" s="23"/>
+      <c r="Z37" s="23"/>
+      <c r="AA37" s="23"/>
+      <c r="AB37" s="23"/>
+      <c r="AC37" s="23"/>
+      <c r="AD37" s="23"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
-      <c r="G38" s="7" t="s">
-        <v>141</v>
-      </c>
+      <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
@@ -2219,8 +2021,22 @@
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="23"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="23"/>
+      <c r="AB38" s="23"/>
+      <c r="AC38" s="23"/>
+      <c r="AD38" s="23"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -2234,10 +2050,38 @@
       <c r="L39" s="7"/>
       <c r="M39" s="7"/>
       <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="23"/>
+      <c r="X39" s="23"/>
+      <c r="Y39" s="23"/>
+      <c r="Z39" s="23"/>
+      <c r="AA39" s="23"/>
+      <c r="AB39" s="23"/>
+      <c r="AC39" s="23"/>
+      <c r="AD39" s="23"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7"/>
@@ -2246,16 +2090,30 @@
       <c r="T40" s="7"/>
       <c r="U40" s="7"/>
       <c r="V40" s="7"/>
-      <c r="W40" s="7"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
-      <c r="Z40" s="7"/>
-      <c r="AA40" s="7"/>
-      <c r="AB40" s="7"/>
-      <c r="AC40" s="7"/>
-      <c r="AD40" s="7"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23"/>
+      <c r="Y40" s="23"/>
+      <c r="Z40" s="23"/>
+      <c r="AA40" s="23"/>
+      <c r="AB40" s="23"/>
+      <c r="AC40" s="23"/>
+      <c r="AD40" s="23"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
@@ -2264,16 +2122,30 @@
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
       <c r="V41" s="7"/>
-      <c r="W41" s="7"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="7"/>
-      <c r="Z41" s="7"/>
-      <c r="AA41" s="7"/>
-      <c r="AB41" s="7"/>
-      <c r="AC41" s="7"/>
-      <c r="AD41" s="7"/>
+      <c r="W41" s="23"/>
+      <c r="X41" s="23"/>
+      <c r="Y41" s="23"/>
+      <c r="Z41" s="23"/>
+      <c r="AA41" s="23"/>
+      <c r="AB41" s="23"/>
+      <c r="AC41" s="23"/>
+      <c r="AD41" s="23"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="7"/>
@@ -2282,16 +2154,17 @@
       <c r="T42" s="7"/>
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
-      <c r="W42" s="7"/>
-      <c r="X42" s="7"/>
-      <c r="Y42" s="7"/>
-      <c r="Z42" s="7"/>
-      <c r="AA42" s="7"/>
-      <c r="AB42" s="7"/>
-      <c r="AC42" s="7"/>
-      <c r="AD42" s="7"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+      <c r="Y42" s="23"/>
+      <c r="Z42" s="23"/>
+      <c r="AA42" s="23"/>
+      <c r="AB42" s="23"/>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="23"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -2323,6 +2196,7 @@
       <c r="AD43" s="23"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -2354,6 +2228,7 @@
       <c r="AD44" s="23"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -32816,361 +32691,20 @@
       <c r="AC996" s="23"/>
       <c r="AD996" s="23"/>
     </row>
-    <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A997" s="7"/>
-      <c r="B997" s="7"/>
-      <c r="C997" s="7"/>
-      <c r="D997" s="7"/>
-      <c r="E997" s="7"/>
-      <c r="F997" s="7"/>
-      <c r="G997" s="7"/>
-      <c r="H997" s="7"/>
-      <c r="I997" s="7"/>
-      <c r="J997" s="7"/>
-      <c r="K997" s="7"/>
-      <c r="L997" s="7"/>
-      <c r="M997" s="7"/>
-      <c r="N997" s="7"/>
-      <c r="O997" s="7"/>
-      <c r="P997" s="7"/>
-      <c r="Q997" s="7"/>
-      <c r="R997" s="7"/>
-      <c r="S997" s="7"/>
-      <c r="T997" s="7"/>
-      <c r="U997" s="7"/>
-      <c r="V997" s="7"/>
-      <c r="W997" s="23"/>
-      <c r="X997" s="23"/>
-      <c r="Y997" s="23"/>
-      <c r="Z997" s="23"/>
-      <c r="AA997" s="23"/>
-      <c r="AB997" s="23"/>
-      <c r="AC997" s="23"/>
-      <c r="AD997" s="23"/>
-    </row>
-    <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A998" s="7"/>
-      <c r="B998" s="7"/>
-      <c r="C998" s="7"/>
-      <c r="D998" s="7"/>
-      <c r="E998" s="7"/>
-      <c r="F998" s="7"/>
-      <c r="G998" s="7"/>
-      <c r="H998" s="7"/>
-      <c r="I998" s="7"/>
-      <c r="J998" s="7"/>
-      <c r="K998" s="7"/>
-      <c r="L998" s="7"/>
-      <c r="M998" s="7"/>
-      <c r="N998" s="7"/>
-      <c r="O998" s="7"/>
-      <c r="P998" s="7"/>
-      <c r="Q998" s="7"/>
-      <c r="R998" s="7"/>
-      <c r="S998" s="7"/>
-      <c r="T998" s="7"/>
-      <c r="U998" s="7"/>
-      <c r="V998" s="7"/>
-      <c r="W998" s="23"/>
-      <c r="X998" s="23"/>
-      <c r="Y998" s="23"/>
-      <c r="Z998" s="23"/>
-      <c r="AA998" s="23"/>
-      <c r="AB998" s="23"/>
-      <c r="AC998" s="23"/>
-      <c r="AD998" s="23"/>
-    </row>
-    <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A999" s="7"/>
-      <c r="B999" s="7"/>
-      <c r="C999" s="7"/>
-      <c r="D999" s="7"/>
-      <c r="E999" s="7"/>
-      <c r="F999" s="7"/>
-      <c r="G999" s="7"/>
-      <c r="H999" s="7"/>
-      <c r="I999" s="7"/>
-      <c r="J999" s="7"/>
-      <c r="K999" s="7"/>
-      <c r="L999" s="7"/>
-      <c r="M999" s="7"/>
-      <c r="N999" s="7"/>
-      <c r="O999" s="7"/>
-      <c r="P999" s="7"/>
-      <c r="Q999" s="7"/>
-      <c r="R999" s="7"/>
-      <c r="S999" s="7"/>
-      <c r="T999" s="7"/>
-      <c r="U999" s="7"/>
-      <c r="V999" s="7"/>
-      <c r="W999" s="23"/>
-      <c r="X999" s="23"/>
-      <c r="Y999" s="23"/>
-      <c r="Z999" s="23"/>
-      <c r="AA999" s="23"/>
-      <c r="AB999" s="23"/>
-      <c r="AC999" s="23"/>
-      <c r="AD999" s="23"/>
-    </row>
-    <row r="1000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1000" s="7"/>
-      <c r="B1000" s="7"/>
-      <c r="C1000" s="7"/>
-      <c r="D1000" s="7"/>
-      <c r="E1000" s="7"/>
-      <c r="F1000" s="7"/>
-      <c r="G1000" s="7"/>
-      <c r="H1000" s="7"/>
-      <c r="I1000" s="7"/>
-      <c r="J1000" s="7"/>
-      <c r="K1000" s="7"/>
-      <c r="L1000" s="7"/>
-      <c r="M1000" s="7"/>
-      <c r="N1000" s="7"/>
-      <c r="O1000" s="7"/>
-      <c r="P1000" s="7"/>
-      <c r="Q1000" s="7"/>
-      <c r="R1000" s="7"/>
-      <c r="S1000" s="7"/>
-      <c r="T1000" s="7"/>
-      <c r="U1000" s="7"/>
-      <c r="V1000" s="7"/>
-      <c r="W1000" s="23"/>
-      <c r="X1000" s="23"/>
-      <c r="Y1000" s="23"/>
-      <c r="Z1000" s="23"/>
-      <c r="AA1000" s="23"/>
-      <c r="AB1000" s="23"/>
-      <c r="AC1000" s="23"/>
-      <c r="AD1000" s="23"/>
-    </row>
-    <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1001" s="7"/>
-      <c r="B1001" s="7"/>
-      <c r="C1001" s="7"/>
-      <c r="D1001" s="7"/>
-      <c r="E1001" s="7"/>
-      <c r="F1001" s="7"/>
-      <c r="G1001" s="7"/>
-      <c r="H1001" s="7"/>
-      <c r="I1001" s="7"/>
-      <c r="J1001" s="7"/>
-      <c r="K1001" s="7"/>
-      <c r="L1001" s="7"/>
-      <c r="M1001" s="7"/>
-      <c r="N1001" s="7"/>
-      <c r="O1001" s="7"/>
-      <c r="P1001" s="7"/>
-      <c r="Q1001" s="7"/>
-      <c r="R1001" s="7"/>
-      <c r="S1001" s="7"/>
-      <c r="T1001" s="7"/>
-      <c r="U1001" s="7"/>
-      <c r="V1001" s="7"/>
-      <c r="W1001" s="23"/>
-      <c r="X1001" s="23"/>
-      <c r="Y1001" s="23"/>
-      <c r="Z1001" s="23"/>
-      <c r="AA1001" s="23"/>
-      <c r="AB1001" s="23"/>
-      <c r="AC1001" s="23"/>
-      <c r="AD1001" s="23"/>
-    </row>
-    <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1002" s="7"/>
-      <c r="B1002" s="7"/>
-      <c r="C1002" s="7"/>
-      <c r="D1002" s="7"/>
-      <c r="E1002" s="7"/>
-      <c r="F1002" s="7"/>
-      <c r="G1002" s="7"/>
-      <c r="H1002" s="7"/>
-      <c r="I1002" s="7"/>
-      <c r="J1002" s="7"/>
-      <c r="K1002" s="7"/>
-      <c r="L1002" s="7"/>
-      <c r="M1002" s="7"/>
-      <c r="N1002" s="7"/>
-      <c r="O1002" s="7"/>
-      <c r="P1002" s="7"/>
-      <c r="Q1002" s="7"/>
-      <c r="R1002" s="7"/>
-      <c r="S1002" s="7"/>
-      <c r="T1002" s="7"/>
-      <c r="U1002" s="7"/>
-      <c r="V1002" s="7"/>
-      <c r="W1002" s="23"/>
-      <c r="X1002" s="23"/>
-      <c r="Y1002" s="23"/>
-      <c r="Z1002" s="23"/>
-      <c r="AA1002" s="23"/>
-      <c r="AB1002" s="23"/>
-      <c r="AC1002" s="23"/>
-      <c r="AD1002" s="23"/>
-    </row>
-    <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1003" s="7"/>
-      <c r="B1003" s="7"/>
-      <c r="C1003" s="7"/>
-      <c r="D1003" s="7"/>
-      <c r="E1003" s="7"/>
-      <c r="F1003" s="7"/>
-      <c r="G1003" s="7"/>
-      <c r="H1003" s="7"/>
-      <c r="I1003" s="7"/>
-      <c r="J1003" s="7"/>
-      <c r="K1003" s="7"/>
-      <c r="L1003" s="7"/>
-      <c r="M1003" s="7"/>
-      <c r="N1003" s="7"/>
-      <c r="O1003" s="7"/>
-      <c r="P1003" s="7"/>
-      <c r="Q1003" s="7"/>
-      <c r="R1003" s="7"/>
-      <c r="S1003" s="7"/>
-      <c r="T1003" s="7"/>
-      <c r="U1003" s="7"/>
-      <c r="V1003" s="7"/>
-      <c r="W1003" s="23"/>
-      <c r="X1003" s="23"/>
-      <c r="Y1003" s="23"/>
-      <c r="Z1003" s="23"/>
-      <c r="AA1003" s="23"/>
-      <c r="AB1003" s="23"/>
-      <c r="AC1003" s="23"/>
-      <c r="AD1003" s="23"/>
-    </row>
-    <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1004" s="7"/>
-      <c r="B1004" s="7"/>
-      <c r="C1004" s="7"/>
-      <c r="D1004" s="7"/>
-      <c r="E1004" s="7"/>
-      <c r="F1004" s="7"/>
-      <c r="G1004" s="7"/>
-      <c r="H1004" s="7"/>
-      <c r="I1004" s="7"/>
-      <c r="J1004" s="7"/>
-      <c r="K1004" s="7"/>
-      <c r="L1004" s="7"/>
-      <c r="M1004" s="7"/>
-      <c r="N1004" s="7"/>
-      <c r="O1004" s="7"/>
-      <c r="P1004" s="7"/>
-      <c r="Q1004" s="7"/>
-      <c r="R1004" s="7"/>
-      <c r="S1004" s="7"/>
-      <c r="T1004" s="7"/>
-      <c r="U1004" s="7"/>
-      <c r="V1004" s="7"/>
-      <c r="W1004" s="23"/>
-      <c r="X1004" s="23"/>
-      <c r="Y1004" s="23"/>
-      <c r="Z1004" s="23"/>
-      <c r="AA1004" s="23"/>
-      <c r="AB1004" s="23"/>
-      <c r="AC1004" s="23"/>
-      <c r="AD1004" s="23"/>
-    </row>
-    <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1005" s="7"/>
-      <c r="B1005" s="7"/>
-      <c r="C1005" s="7"/>
-      <c r="D1005" s="7"/>
-      <c r="E1005" s="7"/>
-      <c r="F1005" s="7"/>
-      <c r="G1005" s="7"/>
-      <c r="H1005" s="7"/>
-      <c r="I1005" s="7"/>
-      <c r="J1005" s="7"/>
-      <c r="K1005" s="7"/>
-      <c r="L1005" s="7"/>
-      <c r="M1005" s="7"/>
-      <c r="N1005" s="7"/>
-      <c r="O1005" s="7"/>
-      <c r="P1005" s="7"/>
-      <c r="Q1005" s="7"/>
-      <c r="R1005" s="7"/>
-      <c r="S1005" s="7"/>
-      <c r="T1005" s="7"/>
-      <c r="U1005" s="7"/>
-      <c r="V1005" s="7"/>
-      <c r="W1005" s="23"/>
-      <c r="X1005" s="23"/>
-      <c r="Y1005" s="23"/>
-      <c r="Z1005" s="23"/>
-      <c r="AA1005" s="23"/>
-      <c r="AB1005" s="23"/>
-      <c r="AC1005" s="23"/>
-      <c r="AD1005" s="23"/>
-    </row>
-    <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1006" s="7"/>
-      <c r="B1006" s="7"/>
-      <c r="C1006" s="7"/>
-      <c r="D1006" s="7"/>
-      <c r="E1006" s="7"/>
-      <c r="F1006" s="7"/>
-      <c r="G1006" s="7"/>
-      <c r="H1006" s="7"/>
-      <c r="I1006" s="7"/>
-      <c r="J1006" s="7"/>
-      <c r="K1006" s="7"/>
-      <c r="L1006" s="7"/>
-      <c r="M1006" s="7"/>
-      <c r="N1006" s="7"/>
-      <c r="O1006" s="7"/>
-      <c r="P1006" s="7"/>
-      <c r="Q1006" s="7"/>
-      <c r="R1006" s="7"/>
-      <c r="S1006" s="7"/>
-      <c r="T1006" s="7"/>
-      <c r="U1006" s="7"/>
-      <c r="V1006" s="7"/>
-      <c r="W1006" s="23"/>
-      <c r="X1006" s="23"/>
-      <c r="Y1006" s="23"/>
-      <c r="Z1006" s="23"/>
-      <c r="AA1006" s="23"/>
-      <c r="AB1006" s="23"/>
-      <c r="AC1006" s="23"/>
-      <c r="AD1006" s="23"/>
-    </row>
-    <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1007" s="7"/>
-      <c r="B1007" s="7"/>
-      <c r="C1007" s="7"/>
-      <c r="D1007" s="7"/>
-      <c r="E1007" s="7"/>
-      <c r="F1007" s="7"/>
-      <c r="G1007" s="7"/>
-      <c r="H1007" s="7"/>
-      <c r="I1007" s="7"/>
-      <c r="J1007" s="7"/>
-      <c r="K1007" s="7"/>
-      <c r="L1007" s="7"/>
-      <c r="M1007" s="7"/>
-      <c r="N1007" s="7"/>
-      <c r="O1007" s="7"/>
-      <c r="P1007" s="7"/>
-      <c r="Q1007" s="7"/>
-      <c r="R1007" s="7"/>
-      <c r="S1007" s="7"/>
-      <c r="T1007" s="7"/>
-      <c r="U1007" s="7"/>
-      <c r="V1007" s="7"/>
-      <c r="W1007" s="23"/>
-      <c r="X1007" s="23"/>
-      <c r="Y1007" s="23"/>
-      <c r="Z1007" s="23"/>
-      <c r="AA1007" s="23"/>
-      <c r="AB1007" s="23"/>
-      <c r="AC1007" s="23"/>
-      <c r="AD1007" s="23"/>
-    </row>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A22:Q22"/>
+    <mergeCell ref="A11:Q11"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>